<commit_message>
Changed A* ignore preconditions to use KB, added documents
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
     <sheet name="Experiments_No_Plan" sheetId="2" r:id="rId2"/>
+    <sheet name="Uninformed planning algorithms" sheetId="3" r:id="rId3"/>
+    <sheet name="Automatic Heuristics" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="56">
   <si>
     <t>P1</t>
   </si>
@@ -275,15 +277,6 @@
 Fly(P1, SFO, JFK)
 Unload(C1, P1, JFK)
  </t>
-  </si>
-  <si>
-    <t>Load(C1, P1, SFO)
-Load(C2, P2, JFK)
-Fly(P1, SFO, JFK)
-Fly(P2, JFK, SFO)
-￼
-Unload(C1, P1, JFK)
-Unload(C2, P2, SFO)</t>
   </si>
   <si>
     <t>Load(C1, P1, SFO)
@@ -342,18 +335,6 @@
 Fly(P1, SFO, JFK)
 Fly(P2, JFK, SFO)
 Fly(P3, ATL, SFO)
-Unload(C3, P3, SFO)
-Unload(C1, P1, JFK)
-Unload(C2, P2, SFO)</t>
-  </si>
-  <si>
-    <t>Load(C1, P1, SFO)
-Load(C2, P2, JFK)
-Load(C3, P3, ATL)
-Fly(P1, SFO, JFK)
-Fly(P2, JFK, SFO)
-Fly(P3, ATL, SFO)
-￼
 Unload(C3, P3, SFO)
 Unload(C1, P1, JFK)
 Unload(C2, P2, SFO)</t>
@@ -400,12 +381,69 @@
   <si>
     <t>Time(s)</t>
   </si>
+  <si>
+    <t>Num of actions</t>
+  </si>
+  <si>
+    <t>20+</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Optimal?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>no *</t>
+  </si>
+  <si>
+    <t>*Note: didn't finished under 10 min, which makes them "Non Optimal" according to the asssumptions of the project.</t>
+  </si>
+  <si>
+    <t>Load(C1, P1, SFO)
+Fly(P1, SFO, JFK)
+Unload(C1, P1, JFK)
+Load(C2, P2, JFK)
+Fly(P2, JFK, SFO)
+Unload(C2, P2, SFO)</t>
+  </si>
+  <si>
+    <t>Load(C3, P3, ATL)
+Fly(P3, ATL, SFO)
+Unload(C3, P3, SFO)
+Load(C1, P1, SFO)
+Fly(P1, SFO, JFK)
+Unload(C1, P1, JFK)
+Load(C2, P2, JFK)
+Fly(P2, JFK, SFO)
+Unload(C2, P2, SFO)</t>
+  </si>
+  <si>
+    <t>Load(C2, P2, JFK)
+Fly(P2, JFK, ORD)
+Load(C4, P2, ORD)
+Fly(P2, ORD, SFO)
+Unload(C4, P2, SFO)
+Load(C1, P1, SFO)
+Fly(P1, SFO, ATL)
+Load(C3, P1, ATL)
+Fly(P1, ATL, JFK)
+Unload(C3, P1, JFK)
+Unload(C1, P1, JFK)
+Unload(C2, P2, SFO)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,16 +451,68 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -445,11 +535,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,13 +610,65 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="I10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,20 +963,20 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
-    <col min="12" max="12" width="28.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.42578125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="26" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="14" width="28.28515625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="26.42578125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -789,20 +986,20 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="1"/>
+      <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -816,53 +1013,62 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="s">
         <v>4</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>5</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>6</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="180" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>43</v>
       </c>
       <c r="D3">
@@ -871,47 +1077,56 @@
       <c r="E3">
         <v>180</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="9">
         <v>5.9343E-2</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="8">
+        <v>6</v>
+      </c>
+      <c r="I3" s="11">
         <v>3343</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>4609</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>30509</v>
       </c>
-      <c r="K3">
+      <c r="L3" s="11">
         <v>17.309999999999999</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M3">
+      <c r="N3" s="10">
+        <v>9</v>
+      </c>
+      <c r="O3" s="15">
         <v>14663</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>18098</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>129631</v>
       </c>
-      <c r="P3">
+      <c r="R3" s="15">
         <v>127.23</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" s="13">
+        <v>12</v>
+      </c>
+      <c r="U3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -933,8 +1148,8 @@
       <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>17</v>
+      <c r="H4" s="8">
+        <v>6</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>17</v>
@@ -952,7 +1167,7 @@
         <v>17</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>17</v>
@@ -963,15 +1178,24 @@
       <c r="Q4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="180" x14ac:dyDescent="0.25">
+      <c r="R4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>12</v>
       </c>
       <c r="D5">
@@ -986,41 +1210,50 @@
       <c r="G5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
+        <v>12</v>
+      </c>
+      <c r="I5">
         <v>582</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>583</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5211</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>4.5199999999999996</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M5">
+      <c r="N5" s="3">
+        <v>20</v>
+      </c>
+      <c r="O5">
         <v>627</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>628</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>5176</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>4.45</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="S5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" s="3">
+        <v>20</v>
+      </c>
+      <c r="U5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1042,26 +1275,26 @@
       <c r="G6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6">
         <v>222719</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2053741</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2054119</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1382</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" t="s">
-        <v>17</v>
+      <c r="N6" s="2">
+        <v>20</v>
       </c>
       <c r="O6" t="s">
         <v>17</v>
@@ -1069,18 +1302,27 @@
       <c r="P6" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="180" x14ac:dyDescent="0.25">
+      <c r="T6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>55</v>
       </c>
       <c r="D7">
@@ -1095,38 +1337,47 @@
       <c r="G7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="8">
+        <v>6</v>
+      </c>
+      <c r="I7" s="11">
         <v>4853</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>4855</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>44041</v>
       </c>
-      <c r="K7">
+      <c r="L7" s="11">
         <v>50.722999999999999</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M7">
+      <c r="N7" s="10">
+        <v>9</v>
+      </c>
+      <c r="O7">
         <v>18223</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>18225</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>159618</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>510.63400000000001</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+      <c r="T7" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1146,28 +1397,28 @@
         <v>3.202</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="12">
+        <v>69347731</v>
+      </c>
+      <c r="J8">
+        <v>69347732</v>
+      </c>
+      <c r="K8">
+        <v>625574973</v>
+      </c>
+      <c r="L8">
+        <v>190736.109</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H8">
-        <v>69347731</v>
-      </c>
-      <c r="I8">
-        <v>69347732</v>
-      </c>
-      <c r="J8">
-        <v>625574973</v>
-      </c>
-      <c r="K8">
-        <v>190736.109</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>17</v>
+      <c r="N8" s="10">
+        <v>9</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>17</v>
@@ -1176,17 +1427,26 @@
         <v>17</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="345" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="345" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <v>7</v>
       </c>
       <c r="D9">
@@ -1195,44 +1455,53 @@
       <c r="E9">
         <v>28</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="9">
         <v>6.8799999999999998E-3</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="8">
+        <v>6</v>
+      </c>
+      <c r="I9">
         <v>998</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1000</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>8982</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>9.0373999999999999</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M9">
+      <c r="M9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="2">
+        <v>20</v>
+      </c>
+      <c r="O9">
         <v>5578</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>5580</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>49150</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>159.34800000000001</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="180" x14ac:dyDescent="0.25">
+      <c r="S9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T9" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1252,40 +1521,49 @@
         <v>0.10929999999999999</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10">
+        <v>36</v>
+      </c>
+      <c r="H10" s="8">
+        <v>6</v>
+      </c>
+      <c r="I10">
         <v>4853</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>4855</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>44041</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>53.018999999999998</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10">
+      <c r="M10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="10">
+        <v>9</v>
+      </c>
+      <c r="O10">
         <v>18223</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>18225</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>159618</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>683.33169999999996</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="150" x14ac:dyDescent="0.25">
+      <c r="T10" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1293,56 +1571,68 @@
         <v>27</v>
       </c>
       <c r="C11">
+        <v>41</v>
+      </c>
+      <c r="D11">
+        <v>43</v>
+      </c>
+      <c r="E11">
+        <v>170</v>
+      </c>
+      <c r="F11">
+        <v>7.8030000000000002E-2</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="8">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>1506</v>
+      </c>
+      <c r="J11">
+        <v>1508</v>
+      </c>
+      <c r="K11">
+        <v>13820</v>
+      </c>
+      <c r="L11">
+        <v>19.478999999999999</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="10">
+        <v>9</v>
+      </c>
+      <c r="O11" s="15">
+        <v>5118</v>
+      </c>
+      <c r="P11">
+        <v>5120</v>
+      </c>
+      <c r="Q11">
+        <v>45650</v>
+      </c>
+      <c r="R11" s="15">
+        <v>125.953</v>
+      </c>
+      <c r="S11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D11">
-        <v>57</v>
-      </c>
-      <c r="E11">
-        <v>224</v>
-      </c>
-      <c r="F11">
-        <v>0.13328000000000001</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11">
-        <v>4853</v>
-      </c>
-      <c r="I11">
-        <v>4855</v>
-      </c>
-      <c r="J11">
-        <v>44041</v>
-      </c>
-      <c r="K11">
-        <v>61.241</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M11">
-        <v>18223</v>
-      </c>
-      <c r="N11">
-        <v>18225</v>
-      </c>
-      <c r="O11">
-        <v>159618</v>
-      </c>
-      <c r="P11">
-        <v>686.49099999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+      <c r="T11" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
         <v>41</v>
       </c>
       <c r="D12">
@@ -1351,32 +1641,32 @@
       <c r="E12">
         <v>167</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="9">
         <v>14.97</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="8">
+        <v>6</v>
+      </c>
+      <c r="I12" s="11">
         <v>2927</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>2929</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>26804</v>
       </c>
-      <c r="K12">
+      <c r="L12" s="12">
         <v>35171</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" t="s">
-        <v>17</v>
+      <c r="M12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" s="10">
+        <v>9</v>
       </c>
       <c r="O12" t="s">
         <v>17</v>
@@ -1384,14 +1674,23 @@
       <c r="P12" t="s">
         <v>17</v>
       </c>
-      <c r="Q12" s="3" t="s">
-        <v>44</v>
+      <c r="Q12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="I1:L1"/>
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1404,7 +1703,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="M11" activeCellId="4" sqref="E11 F11 I11 J11 M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,67 +1724,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>46</v>
+      <c r="M2" s="18" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1545,28 +1844,28 @@
       <c r="E4" s="5">
         <v>1.1060000000000001</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1721,16 +2020,16 @@
       <c r="I8" s="5">
         <v>190736.109</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="8" t="s">
+      <c r="J8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1821,40 +2120,40 @@
         <v>27</v>
       </c>
       <c r="B11" s="5">
-        <v>55</v>
-      </c>
-      <c r="C11" s="5">
-        <v>57</v>
-      </c>
-      <c r="D11" s="5">
-        <v>224</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.13328000000000001</v>
-      </c>
-      <c r="F11" s="5">
-        <v>4853</v>
-      </c>
-      <c r="G11" s="5">
-        <v>4855</v>
-      </c>
-      <c r="H11" s="5">
-        <v>44041</v>
-      </c>
-      <c r="I11" s="5">
-        <v>61.241</v>
-      </c>
-      <c r="J11" s="5">
-        <v>18223</v>
-      </c>
-      <c r="K11" s="5">
-        <v>18225</v>
-      </c>
-      <c r="L11" s="5">
-        <v>159618</v>
-      </c>
-      <c r="M11" s="5">
-        <v>686.49099999999999</v>
+        <v>41</v>
+      </c>
+      <c r="C11">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>170</v>
+      </c>
+      <c r="E11">
+        <v>7.8030000000000002E-2</v>
+      </c>
+      <c r="F11">
+        <v>1506</v>
+      </c>
+      <c r="G11">
+        <v>1508</v>
+      </c>
+      <c r="H11">
+        <v>13820</v>
+      </c>
+      <c r="I11">
+        <v>19.478999999999999</v>
+      </c>
+      <c r="J11">
+        <v>5118</v>
+      </c>
+      <c r="K11">
+        <v>5120</v>
+      </c>
+      <c r="L11">
+        <v>45650</v>
+      </c>
+      <c r="M11">
+        <v>125.953</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1900,11 +2199,530 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6">
+        <v>43</v>
+      </c>
+      <c r="D3" s="6">
+        <v>5.9343E-2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3343</v>
+      </c>
+      <c r="G3" s="6">
+        <v>17.309999999999999</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="6">
+        <v>14663</v>
+      </c>
+      <c r="J3" s="6">
+        <v>127.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1458</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="6">
+        <v>582</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="6">
+        <v>627</v>
+      </c>
+      <c r="J5" s="6">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6">
+        <v>101</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.18490000000000001</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="6">
+        <v>222719</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1382</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="6">
+        <v>55</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.12889999999999999</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="6">
+        <v>4853</v>
+      </c>
+      <c r="G7" s="6">
+        <v>50.722999999999999</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="6">
+        <v>18223</v>
+      </c>
+      <c r="J7" s="6">
+        <v>510.63400000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="6">
+        <v>4229</v>
+      </c>
+      <c r="D8" s="6">
+        <v>3.202</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="6">
+        <v>69347731</v>
+      </c>
+      <c r="G8" s="6">
+        <v>190736.109</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="6">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>6.8799999999999998E-3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="6">
+        <v>998</v>
+      </c>
+      <c r="G9" s="6">
+        <v>9.0373999999999999</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5578</v>
+      </c>
+      <c r="J9" s="6">
+        <v>159.34800000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6">
+        <v>55</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.10929999999999999</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="6">
+        <v>4853</v>
+      </c>
+      <c r="G3" s="6">
+        <v>53.018999999999998</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="6">
+        <v>18223</v>
+      </c>
+      <c r="J3" s="6">
+        <v>683.33169999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="6">
+        <v>41</v>
+      </c>
+      <c r="D4" s="6">
+        <v>7.8030000000000002E-2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1506</v>
+      </c>
+      <c r="G4" s="6">
+        <v>19.478999999999999</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="6">
+        <v>5118</v>
+      </c>
+      <c r="J4" s="6">
+        <v>125.953</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6">
+        <v>41</v>
+      </c>
+      <c r="D5" s="6">
+        <v>14.97</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="6">
+        <v>2927</v>
+      </c>
+      <c r="G5" s="6">
+        <v>35171</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="A6:J6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added last details from runs and plan lenghts
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego.s\Google Drive\Udacity\AIND_Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego.s\Google Drive\Udacity\AIND_Planning_NewV\AIND-Planning-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="56">
   <si>
     <t>P1</t>
   </si>
@@ -268,15 +268,6 @@
 Unload(C3, P1, JFK)
 Unload(C1, P1, JFK)
 Unload(C2, P2, SFO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load(C2, P2, JFK)
-Fly(P2, JFK, SFO)
-Unload(C2, P2, SFO)
-Load(C1, P1, SFO)
-Fly(P1, SFO, JFK)
-Unload(C1, P1, JFK)
- </t>
   </si>
   <si>
     <t>Load(C1, P1, SFO)
@@ -336,17 +327,6 @@
 Fly(P2, JFK, SFO)
 Fly(P3, ATL, SFO)
 Unload(C3, P3, SFO)
-Unload(C1, P1, JFK)
-Unload(C2, P2, SFO)</t>
-  </si>
-  <si>
-    <t>Load(C3, P3, ATL)
-Fly(P3, ATL, SFO)
-Unload(C3, P3, SFO)
-Load(C1, P1, SFO)
-Load(C2, P2, JFK)
-Fly(P1, SFO, JFK)
-Fly(P2, JFK, SFO)
 Unload(C1, P1, JFK)
 Unload(C2, P2, SFO)</t>
   </si>
@@ -397,15 +377,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>no *</t>
-  </si>
-  <si>
-    <t>*Note: didn't finished under 10 min, which makes them "Non Optimal" according to the asssumptions of the project.</t>
-  </si>
-  <si>
     <t>Load(C1, P1, SFO)
 Fly(P1, SFO, JFK)
 Unload(C1, P1, JFK)
@@ -438,23 +409,55 @@
 Unload(C1, P1, JFK)
 Unload(C2, P2, SFO)</t>
   </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load(C1, P1, SFO)
+Fly(P1, SFO, JFK)
+Load(C2, P2, JFK)
+Fly(P2, JFK, SFO)
+Unload(C1, P1, JFK)
+Unload(C2, P2, SFO)
+ </t>
+  </si>
+  <si>
+    <t>Load(C1, P1, SFO)
+Fly(P1, SFO, JFK)
+Load(C2, P2, JFK)
+Fly(P2, JFK, SFO)
+Load(C3, P3, ATL)
+Fly(P3, ATL, SFO)
+Unload(C3, P3, SFO)
+Unload(C1, P1, JFK)
+Unload(C2, P2, SFO)</t>
+  </si>
+  <si>
+    <t>Plan Length</t>
+  </si>
+  <si>
+    <t>Load(C2, P2, JFK)
+Fly(P2, JFK, ORD)
+Load(C4, P2, ORD)
+Fly(P2, ORD, SFO)
+Load(C1, P1, SFO)
+Fly(P1, SFO, ATL)
+Load(C3, P1, ATL)
+Fly(P1, ATL, JFK)
+Unload(C4, P2, SFO)
+Unload(C3, P1, JFK)
+Unload(C1, P1, JFK)
+Unload(C2, P2, SFO)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -467,8 +470,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +526,16 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -576,29 +603,36 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -633,8 +667,26 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -646,32 +698,33 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -952,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,16 +1016,16 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="8" width="26" style="3" customWidth="1"/>
+    <col min="7" max="8" width="26" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="14" width="28.28515625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="28.28515625" style="2" customWidth="1"/>
     <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="26.42578125" style="3" customWidth="1"/>
+    <col min="19" max="20" width="26.42578125" style="2" customWidth="1"/>
     <col min="21" max="21" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -980,24 +1033,24 @@
       <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="I1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="O1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1013,13 +1066,13 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>45</v>
+      <c r="H2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
@@ -1033,11 +1086,11 @@
       <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>45</v>
+      <c r="N2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="O2" t="s">
         <v>4</v>
@@ -1051,11 +1104,11 @@
       <c r="R2" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>45</v>
+      <c r="T2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="U2" t="s">
         <v>16</v>
@@ -1068,7 +1121,7 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>43</v>
       </c>
       <c r="D3">
@@ -1077,16 +1130,16 @@
       <c r="E3">
         <v>180</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>5.9343E-2</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="8">
-        <v>6</v>
-      </c>
-      <c r="I3" s="11">
+      <c r="H3" s="7">
+        <v>6</v>
+      </c>
+      <c r="I3" s="10">
         <v>3343</v>
       </c>
       <c r="J3">
@@ -1095,16 +1148,16 @@
       <c r="K3">
         <v>30509</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>17.309999999999999</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <v>9</v>
       </c>
-      <c r="O3" s="15">
+      <c r="O3" s="14">
         <v>14663</v>
       </c>
       <c r="P3">
@@ -1113,13 +1166,13 @@
       <c r="Q3">
         <v>129631</v>
       </c>
-      <c r="R3" s="15">
+      <c r="R3" s="14">
         <v>127.23</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="S3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="13">
+      <c r="T3" s="12">
         <v>12</v>
       </c>
       <c r="U3" t="s">
@@ -1145,47 +1198,47 @@
       <c r="F4">
         <v>1.1060000000000001</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="8">
-        <v>6</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>47</v>
+      <c r="H4" s="7">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="180" x14ac:dyDescent="0.25">
@@ -1195,7 +1248,7 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>12</v>
       </c>
       <c r="D5">
@@ -1207,10 +1260,10 @@
       <c r="F5">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>12</v>
       </c>
       <c r="I5">
@@ -1225,10 +1278,10 @@
       <c r="L5">
         <v>4.5199999999999996</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>20</v>
       </c>
       <c r="O5">
@@ -1243,10 +1296,10 @@
       <c r="R5">
         <v>4.45</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="2">
         <v>20</v>
       </c>
       <c r="U5" t="s">
@@ -1272,11 +1325,11 @@
       <c r="F6">
         <v>0.18490000000000001</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>46</v>
+      <c r="H6" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="I6">
         <v>222719</v>
@@ -1290,10 +1343,10 @@
       <c r="L6">
         <v>1382</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <v>20</v>
       </c>
       <c r="O6" t="s">
@@ -1308,11 +1361,11 @@
       <c r="R6" t="s">
         <v>17</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="S6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T6" s="2" t="s">
-        <v>47</v>
+      <c r="T6" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="180" x14ac:dyDescent="0.25">
@@ -1322,7 +1375,7 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>55</v>
       </c>
       <c r="D7">
@@ -1334,13 +1387,13 @@
       <c r="F7">
         <v>0.12889999999999999</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="8">
-        <v>6</v>
-      </c>
-      <c r="I7" s="11">
+      <c r="H7" s="7">
+        <v>6</v>
+      </c>
+      <c r="I7" s="10">
         <v>4853</v>
       </c>
       <c r="J7">
@@ -1349,13 +1402,13 @@
       <c r="K7">
         <v>44041</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>50.722999999999999</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="9">
         <v>9</v>
       </c>
       <c r="O7">
@@ -1370,10 +1423,10 @@
       <c r="R7">
         <v>510.63400000000001</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="12">
         <v>12</v>
       </c>
     </row>
@@ -1396,13 +1449,13 @@
       <c r="F8">
         <v>3.202</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="8">
-        <v>6</v>
-      </c>
-      <c r="I8" s="12">
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="7">
+        <v>6</v>
+      </c>
+      <c r="I8" s="11">
         <v>69347731</v>
       </c>
       <c r="J8">
@@ -1414,29 +1467,29 @@
       <c r="L8">
         <v>190736.109</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N8" s="10">
+      <c r="M8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" s="9">
         <v>9</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>47</v>
+      <c r="O8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="345" x14ac:dyDescent="0.25">
@@ -1446,7 +1499,7 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>7</v>
       </c>
       <c r="D9">
@@ -1455,13 +1508,13 @@
       <c r="E9">
         <v>28</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>6.8799999999999998E-3</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>6</v>
       </c>
       <c r="I9">
@@ -1476,10 +1529,10 @@
       <c r="L9">
         <v>9.0373999999999999</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="M9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9" s="1">
         <v>20</v>
       </c>
       <c r="O9">
@@ -1494,10 +1547,10 @@
       <c r="R9">
         <v>159.34800000000001</v>
       </c>
-      <c r="S9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T9" s="2">
+      <c r="S9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T9" s="1">
         <v>20</v>
       </c>
     </row>
@@ -1520,10 +1573,10 @@
       <c r="F10">
         <v>0.10929999999999999</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="8">
+      <c r="G10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="7">
         <v>6</v>
       </c>
       <c r="I10">
@@ -1538,10 +1591,10 @@
       <c r="L10">
         <v>53.018999999999998</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="10">
+      <c r="M10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="9">
         <v>9</v>
       </c>
       <c r="O10">
@@ -1556,10 +1609,10 @@
       <c r="R10">
         <v>683.33169999999996</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="S10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T10" s="13">
+      <c r="T10" s="12">
         <v>12</v>
       </c>
     </row>
@@ -1582,10 +1635,10 @@
       <c r="F11">
         <v>7.8030000000000002E-2</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="8">
+      <c r="G11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="7">
         <v>6</v>
       </c>
       <c r="I11">
@@ -1600,13 +1653,13 @@
       <c r="L11">
         <v>19.478999999999999</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N11" s="10">
+      <c r="M11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="9">
         <v>9</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="14">
         <v>5118</v>
       </c>
       <c r="P11">
@@ -1615,76 +1668,76 @@
       <c r="Q11">
         <v>45650</v>
       </c>
-      <c r="R11" s="15">
+      <c r="R11" s="14">
         <v>125.953</v>
       </c>
-      <c r="S11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="T11" s="14">
+      <c r="S11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T11" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="9">
-        <v>41</v>
+      <c r="C12" s="8">
+        <v>11</v>
       </c>
       <c r="D12">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E12">
-        <v>167</v>
-      </c>
-      <c r="F12" s="9">
-        <v>14.97</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="8">
-        <v>6</v>
-      </c>
-      <c r="I12" s="11">
-        <v>2927</v>
+        <v>50</v>
+      </c>
+      <c r="F12" s="8">
+        <v>3.26</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="7">
+        <v>6</v>
+      </c>
+      <c r="I12" s="10">
+        <v>86</v>
       </c>
       <c r="J12">
-        <v>2929</v>
+        <v>88</v>
       </c>
       <c r="K12">
-        <v>26804</v>
-      </c>
-      <c r="L12" s="12">
-        <v>35171</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N12" s="10">
+        <v>841</v>
+      </c>
+      <c r="L12" s="10">
+        <v>820.67700000000002</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" s="9">
         <v>9</v>
       </c>
-      <c r="O12" t="s">
-        <v>17</v>
-      </c>
-      <c r="P12" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>17</v>
-      </c>
-      <c r="R12" t="s">
-        <v>17</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>47</v>
+      <c r="O12">
+        <v>318</v>
+      </c>
+      <c r="P12">
+        <v>320</v>
+      </c>
+      <c r="Q12">
+        <v>2934</v>
+      </c>
+      <c r="R12">
+        <v>5277.9</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T12" s="2">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1700,10 +1753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" activeCellId="4" sqref="E11 F11 I11 J11 M11"/>
+      <selection activeCell="P12" sqref="A1:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,414 +1765,499 @@
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="20" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="20" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="30"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="18"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="18" t="s">
+      <c r="I2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="M2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="N2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>43</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>56</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>180</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="31">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4">
         <v>5.9343E-2</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="4">
         <v>3343</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="4">
         <v>4609</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="4">
         <v>30509</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3" s="31">
+        <v>9</v>
+      </c>
+      <c r="K3" s="32">
         <v>17.309999999999999</v>
       </c>
-      <c r="J3" s="5">
+      <c r="L3" s="4">
         <v>14663</v>
       </c>
-      <c r="K3" s="5">
+      <c r="M3" s="4">
         <v>18098</v>
       </c>
-      <c r="L3" s="5">
+      <c r="N3" s="4">
         <v>129631</v>
       </c>
-      <c r="M3" s="5">
+      <c r="O3" s="4">
         <v>127.23</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="P3" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1458</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1459</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>5960</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="31">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4">
         <v>1.1060000000000001</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>13</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>48</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="36">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="4">
         <v>582</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="4">
         <v>583</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="4">
         <v>5211</v>
       </c>
-      <c r="I5" s="5">
+      <c r="J5" s="36">
+        <v>575</v>
+      </c>
+      <c r="K5" s="4">
         <v>4.5199999999999996</v>
       </c>
-      <c r="J5" s="5">
+      <c r="L5" s="4">
         <v>627</v>
       </c>
-      <c r="K5" s="5">
+      <c r="M5" s="4">
         <v>628</v>
       </c>
-      <c r="L5" s="5">
+      <c r="N5" s="4">
         <v>5176</v>
       </c>
-      <c r="M5" s="5">
+      <c r="O5" s="4">
         <v>4.45</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="P5" s="36">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>101</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>271</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>414</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="36">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4">
         <v>0.18490000000000001</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="4">
         <v>222719</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="4">
         <v>2053741</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="4">
         <v>2054119</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="36">
+        <v>50</v>
+      </c>
+      <c r="K6" s="4">
         <v>1382</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="L6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>55</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>57</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>224</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="31">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4">
         <v>0.12889999999999999</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="4">
         <v>4853</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="4">
         <v>4855</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="4">
         <v>44041</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J7" s="31">
+        <v>9</v>
+      </c>
+      <c r="K7" s="4">
         <v>50.722999999999999</v>
       </c>
-      <c r="J7" s="5">
+      <c r="L7" s="4">
         <v>18223</v>
       </c>
-      <c r="K7" s="5">
+      <c r="M7" s="4">
         <v>18225</v>
       </c>
-      <c r="L7" s="5">
+      <c r="N7" s="4">
         <v>159618</v>
       </c>
-      <c r="M7" s="5">
+      <c r="O7" s="4">
         <v>510.63400000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="P7" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>4229</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>4230</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>17029</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="31">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4">
         <v>3.202</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="4">
         <v>69347731</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="4">
         <v>69347732</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="4">
         <v>625574973</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8" s="31">
+        <v>9</v>
+      </c>
+      <c r="K8" s="4">
         <v>190736.109</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="L8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>9</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>28</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="31">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4">
         <v>6.8799999999999998E-3</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="4">
         <v>998</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="4">
         <v>1000</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="4">
         <v>8982</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J9" s="36">
+        <v>17</v>
+      </c>
+      <c r="K9" s="4">
         <v>9.0373999999999999</v>
       </c>
-      <c r="J9" s="5">
+      <c r="L9" s="4">
         <v>5578</v>
       </c>
-      <c r="K9" s="5">
+      <c r="M9" s="4">
         <v>5580</v>
       </c>
-      <c r="L9" s="5">
+      <c r="N9" s="4">
         <v>49150</v>
       </c>
-      <c r="M9" s="5">
+      <c r="O9" s="4">
         <v>159.34800000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="P9" s="36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>55</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>57</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>224</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="31">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4">
         <v>0.10929999999999999</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="4">
         <v>4853</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="4">
         <v>4855</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="4">
         <v>44041</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="31">
+        <v>9</v>
+      </c>
+      <c r="K10" s="4">
         <v>53.018999999999998</v>
       </c>
-      <c r="J10" s="5">
+      <c r="L10" s="4">
         <v>18223</v>
       </c>
-      <c r="K10" s="5">
+      <c r="M10" s="4">
         <v>18225</v>
       </c>
-      <c r="L10" s="5">
+      <c r="N10" s="4">
         <v>159618</v>
       </c>
-      <c r="M10" s="5">
+      <c r="O10" s="4">
         <v>683.33169999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="P10" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>41</v>
       </c>
       <c r="C11">
@@ -2128,80 +2266,98 @@
       <c r="D11">
         <v>170</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="31">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4">
         <v>7.8030000000000002E-2</v>
       </c>
-      <c r="F11">
+      <c r="G11" s="4">
         <v>1506</v>
       </c>
-      <c r="G11">
+      <c r="H11" s="4">
         <v>1508</v>
       </c>
-      <c r="H11">
+      <c r="I11" s="4">
         <v>13820</v>
       </c>
-      <c r="I11">
+      <c r="J11" s="31">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4">
         <v>19.478999999999999</v>
       </c>
-      <c r="J11">
+      <c r="L11" s="4">
         <v>5118</v>
       </c>
-      <c r="K11">
+      <c r="M11" s="4">
         <v>5120</v>
       </c>
-      <c r="L11">
+      <c r="N11" s="4">
         <v>45650</v>
       </c>
-      <c r="M11">
+      <c r="O11" s="4">
         <v>125.953</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="P11" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="5">
-        <v>41</v>
-      </c>
-      <c r="C12" s="5">
-        <v>43</v>
-      </c>
-      <c r="D12" s="5">
-        <v>167</v>
-      </c>
-      <c r="E12" s="5">
-        <v>14.97</v>
-      </c>
-      <c r="F12" s="5">
-        <v>2927</v>
-      </c>
-      <c r="G12" s="5">
-        <v>2929</v>
-      </c>
-      <c r="H12" s="5">
-        <v>26804</v>
-      </c>
-      <c r="I12" s="5">
-        <v>35171</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>17</v>
+      <c r="B12" s="4">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4">
+        <v>50</v>
+      </c>
+      <c r="E12" s="31">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3.26</v>
+      </c>
+      <c r="G12" s="4">
+        <v>86</v>
+      </c>
+      <c r="H12" s="4">
+        <v>88</v>
+      </c>
+      <c r="I12" s="4">
+        <v>841</v>
+      </c>
+      <c r="J12" s="31">
+        <v>9</v>
+      </c>
+      <c r="K12" s="4">
+        <v>820.67700000000002</v>
+      </c>
+      <c r="L12" s="4">
+        <v>318</v>
+      </c>
+      <c r="M12" s="4">
+        <v>320</v>
+      </c>
+      <c r="N12" s="4">
+        <v>2934</v>
+      </c>
+      <c r="O12" s="4">
+        <v>5277.9</v>
+      </c>
+      <c r="P12" s="31">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2210,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2222,310 +2378,325 @@
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="20"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="18" t="s">
+      <c r="G2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="J2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="22">
         <v>43</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="22">
         <v>5.9343E-2</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E3" s="31">
+        <v>6</v>
+      </c>
+      <c r="F3" s="22">
         <v>3343</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="22">
         <v>17.309999999999999</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="6">
+      <c r="H3" s="31">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5">
         <v>14663</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="22">
         <v>127.23</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="K3" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="5">
         <v>1458</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1.1060000000000001</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="33">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E5" s="34">
+        <v>12</v>
+      </c>
+      <c r="F5" s="22">
+        <v>582</v>
+      </c>
+      <c r="G5" s="22">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="H5" s="36">
+        <v>575</v>
+      </c>
+      <c r="I5" s="22">
+        <v>627</v>
+      </c>
+      <c r="J5" s="22">
+        <v>4.45</v>
+      </c>
+      <c r="K5" s="36">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="5">
+        <v>101</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.18490000000000001</v>
+      </c>
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="26" t="s">
+      <c r="F6" s="5">
+        <v>222719</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1382</v>
+      </c>
+      <c r="H6" s="21">
         <v>50</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5">
+        <v>55</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.12889999999999999</v>
+      </c>
+      <c r="E7" s="33">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4853</v>
+      </c>
+      <c r="G7" s="5">
+        <v>50.722999999999999</v>
+      </c>
+      <c r="H7" s="31">
+        <v>9</v>
+      </c>
+      <c r="I7" s="5">
+        <v>18223</v>
+      </c>
+      <c r="J7" s="5">
+        <v>510.63400000000001</v>
+      </c>
+      <c r="K7" s="31">
         <v>12</v>
       </c>
-      <c r="D5" s="6">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="6">
-        <v>582</v>
-      </c>
-      <c r="G5" s="6">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="6">
-        <v>627</v>
-      </c>
-      <c r="J5" s="6">
-        <v>4.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4229</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3.202</v>
+      </c>
+      <c r="E8" s="33">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5">
+        <v>69347731</v>
+      </c>
+      <c r="G8" s="5">
+        <v>190736.109</v>
+      </c>
+      <c r="H8" s="31">
+        <v>9</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="22">
+        <v>7</v>
+      </c>
+      <c r="D9" s="22">
+        <v>6.8799999999999998E-3</v>
+      </c>
+      <c r="E9" s="31">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5">
+        <v>998</v>
+      </c>
+      <c r="G9" s="5">
+        <v>9.0373999999999999</v>
+      </c>
+      <c r="H9" s="21">
+        <v>17</v>
+      </c>
+      <c r="I9" s="22">
+        <v>5578</v>
+      </c>
+      <c r="J9" s="5">
+        <v>159.34800000000001</v>
+      </c>
+      <c r="K9" s="36">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="6">
-        <v>101</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.18490000000000001</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="6">
-        <v>222719</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1382</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="6">
-        <v>55</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0.12889999999999999</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="6">
-        <v>4853</v>
-      </c>
-      <c r="G7" s="6">
-        <v>50.722999999999999</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="6">
-        <v>18223</v>
-      </c>
-      <c r="J7" s="6">
-        <v>510.63400000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="6">
-        <v>4229</v>
-      </c>
-      <c r="D8" s="6">
-        <v>3.202</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="6">
-        <v>69347731</v>
-      </c>
-      <c r="G8" s="6">
-        <v>190736.109</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="6">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6">
-        <v>6.8799999999999998E-3</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="6">
-        <v>998</v>
-      </c>
-      <c r="G9" s="6">
-        <v>9.0373999999999999</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="6">
-        <v>5578</v>
-      </c>
-      <c r="J9" s="6">
-        <v>159.34800000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2534,195 +2705,196 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="J1" s="26"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="18" t="s">
+      <c r="G2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="J2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5">
         <v>55</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.10929999999999999</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E3" s="22">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5">
         <v>4853</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>53.018999999999998</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="6">
+      <c r="H3" s="22">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5">
         <v>18223</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>683.33169999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="K3" s="22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="22">
         <v>41</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="22">
         <v>7.8030000000000002E-2</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="22">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5">
         <v>1506</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>19.478999999999999</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="6">
+      <c r="H4" s="22">
+        <v>9</v>
+      </c>
+      <c r="I4" s="5">
         <v>5118</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="22">
         <v>125.953</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="K4" s="22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="6">
-        <v>41</v>
-      </c>
-      <c r="D5" s="6">
-        <v>14.97</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2927</v>
-      </c>
-      <c r="G5" s="6">
-        <v>35171</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
+      <c r="B5" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="22">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3.26</v>
+      </c>
+      <c r="E5" s="22">
+        <v>6</v>
+      </c>
+      <c r="F5" s="22">
+        <v>86</v>
+      </c>
+      <c r="G5" s="23">
+        <v>820.67700000000002</v>
+      </c>
+      <c r="H5" s="22">
+        <v>9</v>
+      </c>
+      <c r="I5" s="22">
+        <v>318</v>
+      </c>
+      <c r="J5" s="23">
+        <v>5277.9089999999997</v>
+      </c>
+      <c r="K5" s="22">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>